<commit_message>
Updated Excel file to include up to 64 bins
</commit_message>
<xml_diff>
--- a/FFT.xlsx
+++ b/FFT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Arduino\FFT VU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EE35C6-5DF3-49CD-B28E-B8C764EF836A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B10BEB-7AA5-4535-BEBC-F0E8B98CFB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34290" yWindow="2895" windowWidth="17280" windowHeight="8970" xr2:uid="{BEB157C1-8120-4C0A-9D11-AA0B8064FCE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BEB157C1-8120-4C0A-9D11-AA0B8064FCE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,9 +261,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -272,9 +270,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -285,16 +281,14 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -303,18 +297,35 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -639,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A83C24-EEAB-4D22-B069-562927E8218D}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,7 +738,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -737,9 +748,9 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11">
         <f>POWER(B7/B6,1/(B9-1))</f>
-        <v>2.1316631165338413</v>
+        <v>1.4236459589857384</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -789,722 +800,1380 @@
     </row>
     <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="7">
+      <c r="B17" s="15">
         <v>0</v>
       </c>
-      <c r="C17" s="8">
-        <f t="shared" ref="C17:C49" si="0">$B$6*POWER($B$11,B17)</f>
+      <c r="C17" s="16">
+        <f t="shared" ref="C17:C80" si="0">$B$6*POWER($B$11,B17)</f>
         <v>80</v>
       </c>
-      <c r="D17" s="8">
-        <f t="shared" ref="D17:D49" si="1">C17/$B$13</f>
+      <c r="D17" s="16">
+        <f t="shared" ref="D17:D80" si="1">C17/$B$13</f>
         <v>2.048</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="16">
         <v>0</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="17">
         <f>((D18-D17)/2)+D17</f>
-        <v>3.2068230313306536</v>
+        <v>2.4818134620013961</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>1</v>
       </c>
-      <c r="C18" s="8">
-        <f t="shared" si="0"/>
-        <v>170.53304932270731</v>
-      </c>
-      <c r="D18" s="8">
-        <f t="shared" si="1"/>
-        <v>4.3656460626613072</v>
-      </c>
-      <c r="E18" s="8">
+      <c r="C18" s="14">
+        <f t="shared" si="0"/>
+        <v>113.89167671885907</v>
+      </c>
+      <c r="D18" s="14">
+        <f t="shared" si="1"/>
+        <v>2.9156269240027921</v>
+      </c>
+      <c r="E18" s="14">
         <f>F17</f>
-        <v>3.2068230313306536</v>
+        <v>2.4818134620013961</v>
       </c>
       <c r="F18" s="5">
         <f>((D19-D18)/2)+D18</f>
-        <v>6.8358663771388013</v>
+        <v>3.5332237061346934</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="8">
-        <f t="shared" si="0"/>
-        <v>363.51901139126153</v>
-      </c>
-      <c r="D19" s="8">
-        <f t="shared" si="1"/>
-        <v>9.3060866916162954</v>
-      </c>
-      <c r="E19" s="8">
-        <f t="shared" ref="E19:E49" si="2">F18</f>
-        <v>6.8358663771388013</v>
+      <c r="C19" s="14">
+        <f t="shared" si="0"/>
+        <v>162.14142532291385</v>
+      </c>
+      <c r="D19" s="14">
+        <f t="shared" si="1"/>
+        <v>4.1508204882665947</v>
+      </c>
+      <c r="E19" s="14">
+        <f t="shared" ref="E19:E81" si="2">F18</f>
+        <v>3.5332237061346934</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" ref="F19:F49" si="3">((D20-D19)/2)+D19</f>
-        <v>14.571764225700598</v>
+        <f t="shared" ref="F19:F81" si="3">((D20-D19)/2)+D19</f>
+        <v>5.0300596514312703</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>3</v>
       </c>
-      <c r="C20" s="8">
-        <f t="shared" si="0"/>
-        <v>774.90006874159758</v>
-      </c>
-      <c r="D20" s="8">
-        <f t="shared" si="1"/>
-        <v>19.837441759784898</v>
-      </c>
-      <c r="E20" s="8">
-        <f t="shared" si="2"/>
-        <v>14.571764225700598</v>
+      <c r="C20" s="14">
+        <f t="shared" si="0"/>
+        <v>230.83198494515415</v>
+      </c>
+      <c r="D20" s="14">
+        <f t="shared" si="1"/>
+        <v>5.909298814595946</v>
+      </c>
+      <c r="E20" s="14">
+        <f t="shared" si="2"/>
+        <v>5.0300596514312703</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="3"/>
-        <v>31.062092342753274</v>
+        <v>7.1610240962173402</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
         <v>4</v>
       </c>
-      <c r="C21" s="8">
-        <f t="shared" si="0"/>
-        <v>1651.825895536002</v>
-      </c>
-      <c r="D21" s="8">
-        <f t="shared" si="1"/>
-        <v>42.286742925721654</v>
-      </c>
-      <c r="E21" s="8">
-        <f t="shared" si="2"/>
-        <v>31.062092342753274</v>
+      <c r="C21" s="14">
+        <f t="shared" si="0"/>
+        <v>328.62302257182557</v>
+      </c>
+      <c r="D21" s="14">
+        <f t="shared" si="1"/>
+        <v>8.4127493778387343</v>
+      </c>
+      <c r="E21" s="14">
+        <f t="shared" si="2"/>
+        <v>7.1610240962173402</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="3"/>
-        <v>66.213916569415417</v>
+        <v>10.194763016779316</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <v>5</v>
       </c>
-      <c r="C22" s="8">
-        <f t="shared" si="0"/>
-        <v>3521.1363364495774</v>
-      </c>
-      <c r="D22" s="8">
-        <f t="shared" si="1"/>
-        <v>90.14109021310918</v>
-      </c>
-      <c r="E22" s="8">
-        <f t="shared" si="2"/>
-        <v>66.213916569415417</v>
+      <c r="C22" s="14">
+        <f t="shared" si="0"/>
+        <v>467.84283811405857</v>
+      </c>
+      <c r="D22" s="14">
+        <f t="shared" si="1"/>
+        <v>11.976776655719899</v>
+      </c>
+      <c r="E22" s="14">
+        <f t="shared" si="2"/>
+        <v>10.194763016779316</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="3"/>
-        <v>141.14576375227182</v>
+        <v>14.513733171655131</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
         <v>6</v>
       </c>
-      <c r="C23" s="8">
-        <f t="shared" si="0"/>
-        <v>7505.8764566966593</v>
-      </c>
-      <c r="D23" s="8">
-        <f t="shared" si="1"/>
-        <v>192.15043729143449</v>
-      </c>
-      <c r="E23" s="8">
-        <f t="shared" si="2"/>
-        <v>141.14576375227182</v>
+      <c r="C23" s="14">
+        <f t="shared" si="0"/>
+        <v>666.04256592149852</v>
+      </c>
+      <c r="D23" s="14">
+        <f t="shared" si="1"/>
+        <v>17.050689687590364</v>
+      </c>
+      <c r="E23" s="14">
+        <f t="shared" si="2"/>
+        <v>14.513733171655131</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="3"/>
-        <v>300.87521864571704</v>
+        <v>20.662417579624091</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="7">
         <v>7</v>
       </c>
-      <c r="C24" s="8">
-        <f t="shared" si="0"/>
-        <v>15999.999999999985</v>
-      </c>
-      <c r="D24" s="8">
-        <f t="shared" si="1"/>
-        <v>409.59999999999962</v>
-      </c>
-      <c r="E24" s="8">
-        <f t="shared" si="2"/>
-        <v>300.87521864571704</v>
+      <c r="C24" s="14">
+        <f t="shared" si="0"/>
+        <v>948.20880748663353</v>
+      </c>
+      <c r="D24" s="14">
+        <f t="shared" si="1"/>
+        <v>24.274145471657818</v>
+      </c>
+      <c r="E24" s="14">
+        <f t="shared" si="2"/>
+        <v>20.662417579624091</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="3"/>
-        <v>641.36460626613018</v>
+        <v>29.415967290107719</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="7">
         <v>8</v>
       </c>
-      <c r="C25" s="8">
-        <f t="shared" si="0"/>
-        <v>34106.609864541431</v>
-      </c>
-      <c r="D25" s="8">
-        <f t="shared" si="1"/>
-        <v>873.12921253226068</v>
-      </c>
-      <c r="E25" s="8">
-        <f t="shared" si="2"/>
-        <v>641.36460626613018</v>
+      <c r="C25" s="14">
+        <f t="shared" si="0"/>
+        <v>1349.9136370530321</v>
+      </c>
+      <c r="D25" s="14">
+        <f t="shared" si="1"/>
+        <v>34.557789108557621</v>
+      </c>
+      <c r="E25" s="14">
+        <f t="shared" si="2"/>
+        <v>29.415967290107719</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="3"/>
-        <v>1367.1732754277591</v>
+        <v>41.87792296221852</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
         <v>9</v>
       </c>
-      <c r="C26" s="8">
-        <f t="shared" si="0"/>
-        <v>72703.802278252246</v>
-      </c>
-      <c r="D26" s="8">
-        <f t="shared" si="1"/>
-        <v>1861.2173383232575</v>
-      </c>
-      <c r="E26" s="8">
-        <f t="shared" si="2"/>
-        <v>1367.1732754277591</v>
+      <c r="C26" s="14">
+        <f t="shared" si="0"/>
+        <v>1921.7990943702898</v>
+      </c>
+      <c r="D26" s="14">
+        <f t="shared" si="1"/>
+        <v>49.198056815879418</v>
+      </c>
+      <c r="E26" s="14">
+        <f t="shared" si="2"/>
+        <v>41.87792296221852</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="3"/>
-        <v>2914.3528451401171</v>
+        <v>59.619335795878456</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
         <v>10</v>
       </c>
-      <c r="C27" s="8">
-        <f t="shared" si="0"/>
-        <v>154980.01374831938</v>
-      </c>
-      <c r="D27" s="8">
-        <f t="shared" si="1"/>
-        <v>3967.4883519569762</v>
-      </c>
-      <c r="E27" s="8">
-        <f t="shared" si="2"/>
-        <v>2914.3528451401171</v>
+      <c r="C27" s="14">
+        <f t="shared" si="0"/>
+        <v>2735.961514682715</v>
+      </c>
+      <c r="D27" s="14">
+        <f t="shared" si="1"/>
+        <v>70.040614775877501</v>
+      </c>
+      <c r="E27" s="14">
+        <f t="shared" si="2"/>
+        <v>59.619335795878456</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="3"/>
-        <v>6212.4184685506498</v>
+        <v>84.876826483216149</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
         <v>11</v>
       </c>
-      <c r="C28" s="8">
-        <f t="shared" si="0"/>
-        <v>330365.17910720012</v>
-      </c>
-      <c r="D28" s="8">
-        <f t="shared" si="1"/>
-        <v>8457.3485851443238</v>
-      </c>
-      <c r="E28" s="8">
-        <f t="shared" si="2"/>
-        <v>6212.4184685506498</v>
+      <c r="C28" s="14">
+        <f t="shared" si="0"/>
+        <v>3895.040554318547</v>
+      </c>
+      <c r="D28" s="14">
+        <f t="shared" si="1"/>
+        <v>99.713038190554798</v>
+      </c>
+      <c r="E28" s="14">
+        <f t="shared" si="2"/>
+        <v>84.876826483216149</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="3"/>
-        <v>13242.783313883072</v>
+        <v>120.83455103436438</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="7">
         <v>12</v>
       </c>
-      <c r="C29" s="8">
-        <f t="shared" si="0"/>
-        <v>704227.26728991489</v>
-      </c>
-      <c r="D29" s="8">
-        <f t="shared" si="1"/>
-        <v>18028.218042621822</v>
-      </c>
-      <c r="E29" s="8">
-        <f t="shared" si="2"/>
-        <v>13242.783313883072</v>
+      <c r="C29" s="14">
+        <f t="shared" si="0"/>
+        <v>5545.1587452411704</v>
+      </c>
+      <c r="D29" s="14">
+        <f t="shared" si="1"/>
+        <v>141.95606387817395</v>
+      </c>
+      <c r="E29" s="14">
+        <f t="shared" si="2"/>
+        <v>120.83455103436438</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="3"/>
-        <v>28229.152750454341</v>
+        <v>172.02562028592882</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="7">
         <v>13</v>
       </c>
-      <c r="C30" s="8">
-        <f t="shared" si="0"/>
-        <v>1501175.2913393304</v>
-      </c>
-      <c r="D30" s="8">
-        <f t="shared" si="1"/>
-        <v>38430.087458286856</v>
-      </c>
-      <c r="E30" s="8">
-        <f t="shared" si="2"/>
-        <v>28229.152750454341</v>
+      <c r="C30" s="14">
+        <f t="shared" si="0"/>
+        <v>7894.3428395970204</v>
+      </c>
+      <c r="D30" s="14">
+        <f t="shared" si="1"/>
+        <v>202.09517669368373</v>
+      </c>
+      <c r="E30" s="14">
+        <f t="shared" si="2"/>
+        <v>172.02562028592882</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="3"/>
-        <v>60175.043729143363</v>
+        <v>244.90357916207768</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="7">
         <v>14</v>
       </c>
-      <c r="C31" s="8">
-        <f t="shared" si="0"/>
-        <v>3199999.9999999949</v>
-      </c>
-      <c r="D31" s="8">
-        <f t="shared" si="1"/>
-        <v>81919.999999999869</v>
-      </c>
-      <c r="E31" s="8">
-        <f t="shared" si="2"/>
-        <v>60175.043729143363</v>
+      <c r="C31" s="14">
+        <f t="shared" si="0"/>
+        <v>11238.749282440298</v>
+      </c>
+      <c r="D31" s="14">
+        <f t="shared" si="1"/>
+        <v>287.71198163047166</v>
+      </c>
+      <c r="E31" s="14">
+        <f t="shared" si="2"/>
+        <v>244.90357916207768</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="3"/>
-        <v>128272.92125322594</v>
+        <v>348.65599081523578</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="7">
         <v>15</v>
       </c>
-      <c r="C32" s="8">
-        <f t="shared" si="0"/>
-        <v>6821321.9729082808</v>
-      </c>
-      <c r="D32" s="8">
-        <f t="shared" si="1"/>
-        <v>174625.842506452</v>
-      </c>
-      <c r="E32" s="8">
-        <f t="shared" si="2"/>
-        <v>128272.92125322594</v>
+      <c r="C32" s="14">
+        <f t="shared" si="0"/>
+        <v>15999.999999999998</v>
+      </c>
+      <c r="D32" s="14">
+        <f t="shared" si="1"/>
+        <v>409.59999999999997</v>
+      </c>
+      <c r="E32" s="14">
+        <f t="shared" si="2"/>
+        <v>348.65599081523578</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" si="3"/>
-        <v>273434.65508555161</v>
+        <v>496.36269240027923</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="7">
         <v>16</v>
       </c>
-      <c r="C33" s="8">
-        <f t="shared" si="0"/>
-        <v>14540760.455650438</v>
-      </c>
-      <c r="D33" s="8">
-        <f t="shared" si="1"/>
-        <v>372243.46766465122</v>
-      </c>
-      <c r="E33" s="8">
-        <f t="shared" si="2"/>
-        <v>273434.65508555161</v>
+      <c r="C33" s="14">
+        <f t="shared" si="0"/>
+        <v>22778.335343771814</v>
+      </c>
+      <c r="D33" s="14">
+        <f t="shared" si="1"/>
+        <v>583.12538480055844</v>
+      </c>
+      <c r="E33" s="14">
+        <f t="shared" si="2"/>
+        <v>496.36269240027923</v>
       </c>
       <c r="F33" s="5">
         <f t="shared" si="3"/>
-        <v>582870.56902802293</v>
+        <v>706.64474122693855</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="7">
         <v>17</v>
       </c>
-      <c r="C34" s="8">
-        <f t="shared" si="0"/>
-        <v>30996002.749663852</v>
-      </c>
-      <c r="D34" s="8">
-        <f t="shared" si="1"/>
-        <v>793497.67039139464</v>
-      </c>
-      <c r="E34" s="8">
-        <f t="shared" si="2"/>
-        <v>582870.56902802293</v>
+      <c r="C34" s="14">
+        <f t="shared" si="0"/>
+        <v>32428.285064582764</v>
+      </c>
+      <c r="D34" s="14">
+        <f t="shared" si="1"/>
+        <v>830.16409765331878</v>
+      </c>
+      <c r="E34" s="14">
+        <f t="shared" si="2"/>
+        <v>706.64474122693855</v>
       </c>
       <c r="F34" s="5">
         <f t="shared" si="3"/>
-        <v>1242483.6937101288</v>
+        <v>1006.011930286254</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="7">
         <v>18</v>
       </c>
-      <c r="C35" s="8">
-        <f t="shared" si="0"/>
-        <v>66073035.821439967</v>
-      </c>
-      <c r="D35" s="8">
-        <f t="shared" si="1"/>
-        <v>1691469.717028863</v>
-      </c>
-      <c r="E35" s="8">
-        <f t="shared" si="2"/>
-        <v>1242483.6937101288</v>
+      <c r="C35" s="14">
+        <f t="shared" si="0"/>
+        <v>46166.396989030829</v>
+      </c>
+      <c r="D35" s="14">
+        <f t="shared" si="1"/>
+        <v>1181.8597629191893</v>
+      </c>
+      <c r="E35" s="14">
+        <f t="shared" si="2"/>
+        <v>1006.011930286254</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" si="3"/>
-        <v>2648556.6627766122</v>
+        <v>1432.2048192434679</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="7">
         <v>19</v>
       </c>
-      <c r="C36" s="8">
-        <f t="shared" si="0"/>
-        <v>140845453.45798287</v>
-      </c>
-      <c r="D36" s="8">
-        <f t="shared" si="1"/>
-        <v>3605643.6085243616</v>
-      </c>
-      <c r="E36" s="8">
-        <f t="shared" si="2"/>
-        <v>2648556.6627766122</v>
+      <c r="C36" s="14">
+        <f t="shared" si="0"/>
+        <v>65724.604514365099</v>
+      </c>
+      <c r="D36" s="14">
+        <f t="shared" si="1"/>
+        <v>1682.5498755677465</v>
+      </c>
+      <c r="E36" s="14">
+        <f t="shared" si="2"/>
+        <v>1432.2048192434679</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="3"/>
-        <v>5645830.5500908634</v>
+        <v>2038.9526033558632</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" s="7">
         <v>20</v>
       </c>
-      <c r="C37" s="8">
-        <f t="shared" si="0"/>
-        <v>300235058.26786584</v>
-      </c>
-      <c r="D37" s="8">
-        <f t="shared" si="1"/>
-        <v>7686017.4916573651</v>
-      </c>
-      <c r="E37" s="8">
-        <f t="shared" si="2"/>
-        <v>5645830.5500908634</v>
+      <c r="C37" s="14">
+        <f t="shared" si="0"/>
+        <v>93568.567622811708</v>
+      </c>
+      <c r="D37" s="14">
+        <f t="shared" si="1"/>
+        <v>2395.3553311439796</v>
+      </c>
+      <c r="E37" s="14">
+        <f t="shared" si="2"/>
+        <v>2038.9526033558632</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="3"/>
-        <v>12035008.745828662</v>
+        <v>2902.7466343310261</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="7">
         <v>21</v>
       </c>
-      <c r="C38" s="8">
-        <f t="shared" si="0"/>
-        <v>639999999.99999845</v>
-      </c>
-      <c r="D38" s="8">
-        <f t="shared" si="1"/>
-        <v>16383999.999999961</v>
-      </c>
-      <c r="E38" s="8">
-        <f t="shared" si="2"/>
-        <v>12035008.745828662</v>
+      <c r="C38" s="14">
+        <f t="shared" si="0"/>
+        <v>133208.51318429969</v>
+      </c>
+      <c r="D38" s="14">
+        <f t="shared" si="1"/>
+        <v>3410.1379375180722</v>
+      </c>
+      <c r="E38" s="14">
+        <f t="shared" si="2"/>
+        <v>2902.7466343310261</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="3"/>
-        <v>25654584.250645161</v>
+        <v>4132.4835159248178</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" s="7">
         <v>22</v>
       </c>
-      <c r="C39" s="8">
-        <f t="shared" si="0"/>
-        <v>1364264394.581655</v>
-      </c>
-      <c r="D39" s="8">
-        <f t="shared" si="1"/>
-        <v>34925168.501290366</v>
-      </c>
-      <c r="E39" s="8">
-        <f t="shared" si="2"/>
-        <v>25654584.250645161</v>
+      <c r="C39" s="14">
+        <f t="shared" si="0"/>
+        <v>189641.76149732672</v>
+      </c>
+      <c r="D39" s="14">
+        <f t="shared" si="1"/>
+        <v>4854.8290943315642</v>
+      </c>
+      <c r="E39" s="14">
+        <f t="shared" si="2"/>
+        <v>4132.4835159248178</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="3"/>
-        <v>54686931.017110273</v>
+        <v>5883.1934580215438</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="7">
         <v>23</v>
       </c>
-      <c r="C40" s="8">
-        <f t="shared" si="0"/>
-        <v>2908152091.130085</v>
-      </c>
-      <c r="D40" s="8">
-        <f t="shared" si="1"/>
-        <v>74448693.53293018</v>
-      </c>
-      <c r="E40" s="8">
-        <f t="shared" si="2"/>
-        <v>54686931.017110273</v>
+      <c r="C40" s="14">
+        <f t="shared" si="0"/>
+        <v>269982.72741060634</v>
+      </c>
+      <c r="D40" s="14">
+        <f t="shared" si="1"/>
+        <v>6911.5578217115226</v>
+      </c>
+      <c r="E40" s="14">
+        <f t="shared" si="2"/>
+        <v>5883.1934580215438</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" si="3"/>
-        <v>116574113.80560449</v>
+        <v>8375.5845924437035</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" s="7">
         <v>24</v>
       </c>
-      <c r="C41" s="8">
-        <f t="shared" si="0"/>
-        <v>6199200549.932765</v>
-      </c>
-      <c r="D41" s="8">
-        <f t="shared" si="1"/>
-        <v>158699534.07827878</v>
-      </c>
-      <c r="E41" s="8">
-        <f t="shared" si="2"/>
-        <v>116574113.80560449</v>
+      <c r="C41" s="14">
+        <f t="shared" si="0"/>
+        <v>384359.81887405796</v>
+      </c>
+      <c r="D41" s="14">
+        <f t="shared" si="1"/>
+        <v>9839.6113631758835</v>
+      </c>
+      <c r="E41" s="14">
+        <f t="shared" si="2"/>
+        <v>8375.5845924437035</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" si="3"/>
-        <v>248496738.74202558</v>
+        <v>11923.867159175692</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
         <v>25</v>
       </c>
-      <c r="C42" s="8">
-        <f t="shared" si="0"/>
-        <v>13214607164.287983</v>
-      </c>
-      <c r="D42" s="8">
-        <f t="shared" si="1"/>
-        <v>338293943.40577239</v>
-      </c>
-      <c r="E42" s="8">
-        <f t="shared" si="2"/>
-        <v>248496738.74202558</v>
+      <c r="C42" s="14">
+        <f t="shared" si="0"/>
+        <v>547192.30293654301</v>
+      </c>
+      <c r="D42" s="14">
+        <f t="shared" si="1"/>
+        <v>14008.1229551755</v>
+      </c>
+      <c r="E42" s="14">
+        <f t="shared" si="2"/>
+        <v>11923.867159175692</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" si="3"/>
-        <v>529711332.55532193</v>
+        <v>16975.365296643231</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" s="7">
         <v>26</v>
       </c>
-      <c r="C43" s="8">
-        <f t="shared" si="0"/>
-        <v>28169090691.596546</v>
-      </c>
-      <c r="D43" s="8">
-        <f t="shared" si="1"/>
-        <v>721128721.70487154</v>
-      </c>
-      <c r="E43" s="8">
-        <f t="shared" si="2"/>
-        <v>529711332.55532193</v>
+      <c r="C43" s="14">
+        <f t="shared" si="0"/>
+        <v>779008.11086370947</v>
+      </c>
+      <c r="D43" s="14">
+        <f t="shared" si="1"/>
+        <v>19942.607638110963</v>
+      </c>
+      <c r="E43" s="14">
+        <f t="shared" si="2"/>
+        <v>16975.365296643231</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="3"/>
-        <v>1129166110.0181718</v>
+        <v>24166.910206872875</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" s="7">
         <v>27</v>
       </c>
-      <c r="C44" s="8">
-        <f t="shared" si="0"/>
-        <v>60047011653.57312</v>
-      </c>
-      <c r="D44" s="8">
-        <f t="shared" si="1"/>
-        <v>1537203498.3314719</v>
-      </c>
-      <c r="E44" s="8">
-        <f t="shared" si="2"/>
-        <v>1129166110.0181718</v>
+      <c r="C44" s="14">
+        <f t="shared" si="0"/>
+        <v>1109031.749048234</v>
+      </c>
+      <c r="D44" s="14">
+        <f t="shared" si="1"/>
+        <v>28391.212775634791</v>
+      </c>
+      <c r="E44" s="14">
+        <f t="shared" si="2"/>
+        <v>24166.910206872875</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" si="3"/>
-        <v>2407001749.1657305</v>
+        <v>34405.124057185763</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" s="7">
         <v>28</v>
       </c>
-      <c r="C45" s="8">
-        <f t="shared" si="0"/>
-        <v>127999999999.99957</v>
-      </c>
-      <c r="D45" s="8">
-        <f t="shared" si="1"/>
-        <v>3276799999.999989</v>
-      </c>
-      <c r="E45" s="8">
-        <f t="shared" si="2"/>
-        <v>2407001749.1657305</v>
+      <c r="C45" s="14">
+        <f t="shared" si="0"/>
+        <v>1578868.567919404</v>
+      </c>
+      <c r="D45" s="14">
+        <f t="shared" si="1"/>
+        <v>40419.035338736743</v>
+      </c>
+      <c r="E45" s="14">
+        <f t="shared" si="2"/>
+        <v>34405.124057185763</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" si="3"/>
-        <v>5130916850.1290283</v>
+        <v>48980.715832415532</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" s="7">
         <v>29</v>
       </c>
-      <c r="C46" s="8">
-        <f t="shared" si="0"/>
-        <v>272852878916.33075</v>
-      </c>
-      <c r="D46" s="8">
-        <f t="shared" si="1"/>
-        <v>6985033700.2580671</v>
-      </c>
-      <c r="E46" s="8">
-        <f t="shared" si="2"/>
-        <v>5130916850.1290283</v>
+      <c r="C46" s="14">
+        <f t="shared" si="0"/>
+        <v>2247749.8564880593</v>
+      </c>
+      <c r="D46" s="14">
+        <f t="shared" si="1"/>
+        <v>57542.39632609432</v>
+      </c>
+      <c r="E46" s="14">
+        <f t="shared" si="2"/>
+        <v>48980.715832415532</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" si="3"/>
-        <v>10937386203.422047</v>
+        <v>69731.198163047156</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" s="7">
         <v>30</v>
       </c>
-      <c r="C47" s="8">
-        <f t="shared" si="0"/>
-        <v>581630418226.0166</v>
-      </c>
-      <c r="D47" s="8">
-        <f t="shared" si="1"/>
-        <v>14889738706.586025</v>
-      </c>
-      <c r="E47" s="8">
-        <f t="shared" si="2"/>
-        <v>10937386203.422047</v>
+      <c r="C47" s="14">
+        <f t="shared" si="0"/>
+        <v>3199999.9999999995</v>
+      </c>
+      <c r="D47" s="14">
+        <f t="shared" si="1"/>
+        <v>81919.999999999985</v>
+      </c>
+      <c r="E47" s="14">
+        <f t="shared" si="2"/>
+        <v>69731.198163047156</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="3"/>
-        <v>23314822761.12088</v>
+        <v>99272.538480055824</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
         <v>31</v>
       </c>
-      <c r="C48" s="8">
-        <f t="shared" si="0"/>
-        <v>1239840109986.552</v>
-      </c>
-      <c r="D48" s="8">
-        <f t="shared" si="1"/>
-        <v>31739906815.655731</v>
-      </c>
-      <c r="E48" s="8">
-        <f t="shared" si="2"/>
-        <v>23314822761.12088</v>
+      <c r="C48" s="14">
+        <f t="shared" si="0"/>
+        <v>4555667.0687543619</v>
+      </c>
+      <c r="D48" s="14">
+        <f t="shared" si="1"/>
+        <v>116625.07696011166</v>
+      </c>
+      <c r="E48" s="14">
+        <f t="shared" si="2"/>
+        <v>99272.538480055824</v>
       </c>
       <c r="F48" s="5">
         <f t="shared" si="3"/>
-        <v>49699347748.405075</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="9">
+        <v>141328.9482453877</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="7">
         <v>32</v>
       </c>
-      <c r="C49" s="10">
-        <f t="shared" si="0"/>
-        <v>2642921432857.5942</v>
-      </c>
-      <c r="D49" s="10">
-        <f t="shared" si="1"/>
-        <v>67658788681.154411</v>
-      </c>
-      <c r="E49" s="10">
-        <f t="shared" si="2"/>
-        <v>49699347748.405075</v>
-      </c>
-      <c r="F49" s="6">
-        <f t="shared" si="3"/>
-        <v>33829394340.577206</v>
-      </c>
+      <c r="C49" s="14">
+        <f t="shared" si="0"/>
+        <v>6485657.0129165528</v>
+      </c>
+      <c r="D49" s="14">
+        <f t="shared" si="1"/>
+        <v>166032.81953066375</v>
+      </c>
+      <c r="E49" s="14">
+        <f t="shared" si="2"/>
+        <v>141328.9482453877</v>
+      </c>
+      <c r="F49" s="5">
+        <f t="shared" si="3"/>
+        <v>201202.38605725078</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50" s="7">
+        <v>33</v>
+      </c>
+      <c r="C50" s="14">
+        <f t="shared" si="0"/>
+        <v>9233279.3978061657</v>
+      </c>
+      <c r="D50" s="14">
+        <f t="shared" si="1"/>
+        <v>236371.95258383785</v>
+      </c>
+      <c r="E50" s="14">
+        <f t="shared" si="2"/>
+        <v>201202.38605725078</v>
+      </c>
+      <c r="F50" s="5">
+        <f t="shared" si="3"/>
+        <v>286440.96384869359</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51" s="7">
+        <v>34</v>
+      </c>
+      <c r="C51" s="14">
+        <f t="shared" si="0"/>
+        <v>13144920.902873021</v>
+      </c>
+      <c r="D51" s="14">
+        <f t="shared" si="1"/>
+        <v>336509.97511354933</v>
+      </c>
+      <c r="E51" s="14">
+        <f t="shared" si="2"/>
+        <v>286440.96384869359</v>
+      </c>
+      <c r="F51" s="5">
+        <f t="shared" si="3"/>
+        <v>407790.52067117265</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52" s="7">
+        <v>35</v>
+      </c>
+      <c r="C52" s="14">
+        <f t="shared" si="0"/>
+        <v>18713713.52456234</v>
+      </c>
+      <c r="D52" s="14">
+        <f t="shared" si="1"/>
+        <v>479071.06622879591</v>
+      </c>
+      <c r="E52" s="14">
+        <f t="shared" si="2"/>
+        <v>407790.52067117265</v>
+      </c>
+      <c r="F52" s="5">
+        <f t="shared" si="3"/>
+        <v>580549.32686620508</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="7">
+        <v>36</v>
+      </c>
+      <c r="C53" s="14">
+        <f t="shared" si="0"/>
+        <v>26641702.636859939</v>
+      </c>
+      <c r="D53" s="14">
+        <f t="shared" si="1"/>
+        <v>682027.58750361437</v>
+      </c>
+      <c r="E53" s="14">
+        <f t="shared" si="2"/>
+        <v>580549.32686620508</v>
+      </c>
+      <c r="F53" s="5">
+        <f t="shared" si="3"/>
+        <v>826496.70318496355</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54" s="7">
+        <v>37</v>
+      </c>
+      <c r="C54" s="14">
+        <f t="shared" si="0"/>
+        <v>37928352.299465343</v>
+      </c>
+      <c r="D54" s="14">
+        <f t="shared" si="1"/>
+        <v>970965.81886631274</v>
+      </c>
+      <c r="E54" s="14">
+        <f t="shared" si="2"/>
+        <v>826496.70318496355</v>
+      </c>
+      <c r="F54" s="5">
+        <f t="shared" si="3"/>
+        <v>1176638.6916043088</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="7">
+        <v>38</v>
+      </c>
+      <c r="C55" s="14">
+        <f t="shared" si="0"/>
+        <v>53996545.482121274</v>
+      </c>
+      <c r="D55" s="14">
+        <f t="shared" si="1"/>
+        <v>1382311.5643423046</v>
+      </c>
+      <c r="E55" s="14">
+        <f t="shared" si="2"/>
+        <v>1176638.6916043088</v>
+      </c>
+      <c r="F55" s="5">
+        <f t="shared" si="3"/>
+        <v>1675116.9184887407</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56" s="7">
+        <v>39</v>
+      </c>
+      <c r="C56" s="14">
+        <f t="shared" si="0"/>
+        <v>76871963.774811596</v>
+      </c>
+      <c r="D56" s="14">
+        <f t="shared" si="1"/>
+        <v>1967922.2726351768</v>
+      </c>
+      <c r="E56" s="14">
+        <f t="shared" si="2"/>
+        <v>1675116.9184887407</v>
+      </c>
+      <c r="F56" s="5">
+        <f t="shared" si="3"/>
+        <v>2384773.4318351382</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57" s="7">
+        <v>40</v>
+      </c>
+      <c r="C57" s="14">
+        <f t="shared" si="0"/>
+        <v>109438460.58730859</v>
+      </c>
+      <c r="D57" s="14">
+        <f t="shared" si="1"/>
+        <v>2801624.5910350997</v>
+      </c>
+      <c r="E57" s="14">
+        <f t="shared" si="2"/>
+        <v>2384773.4318351382</v>
+      </c>
+      <c r="F57" s="5">
+        <f t="shared" si="3"/>
+        <v>3395073.0593286459</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58" s="7">
+        <v>41</v>
+      </c>
+      <c r="C58" s="14">
+        <f t="shared" si="0"/>
+        <v>155801622.17274189</v>
+      </c>
+      <c r="D58" s="14">
+        <f t="shared" si="1"/>
+        <v>3988521.5276221922</v>
+      </c>
+      <c r="E58" s="14">
+        <f t="shared" si="2"/>
+        <v>3395073.0593286459</v>
+      </c>
+      <c r="F58" s="5">
+        <f t="shared" si="3"/>
+        <v>4833382.0413745753</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="7">
+        <v>42</v>
+      </c>
+      <c r="C59" s="14">
+        <f t="shared" si="0"/>
+        <v>221806349.80964684</v>
+      </c>
+      <c r="D59" s="14">
+        <f t="shared" si="1"/>
+        <v>5678242.5551269595</v>
+      </c>
+      <c r="E59" s="14">
+        <f t="shared" si="2"/>
+        <v>4833382.0413745753</v>
+      </c>
+      <c r="F59" s="5">
+        <f t="shared" si="3"/>
+        <v>6881024.8114371542</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="7">
+        <v>43</v>
+      </c>
+      <c r="C60" s="14">
+        <f t="shared" si="0"/>
+        <v>315773713.58388078</v>
+      </c>
+      <c r="D60" s="14">
+        <f t="shared" si="1"/>
+        <v>8083807.067747348</v>
+      </c>
+      <c r="E60" s="14">
+        <f t="shared" si="2"/>
+        <v>6881024.8114371542</v>
+      </c>
+      <c r="F60" s="5">
+        <f t="shared" si="3"/>
+        <v>9796143.1664831061</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61" s="7">
+        <v>44</v>
+      </c>
+      <c r="C61" s="14">
+        <f t="shared" si="0"/>
+        <v>449549971.29761189</v>
+      </c>
+      <c r="D61" s="14">
+        <f t="shared" si="1"/>
+        <v>11508479.265218865</v>
+      </c>
+      <c r="E61" s="14">
+        <f t="shared" si="2"/>
+        <v>9796143.1664831061</v>
+      </c>
+      <c r="F61" s="5">
+        <f t="shared" si="3"/>
+        <v>13946239.632609431</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62" s="7">
+        <v>45</v>
+      </c>
+      <c r="C62" s="14">
+        <f t="shared" si="0"/>
+        <v>639999999.99999988</v>
+      </c>
+      <c r="D62" s="14">
+        <f t="shared" si="1"/>
+        <v>16383999.999999996</v>
+      </c>
+      <c r="E62" s="14">
+        <f t="shared" si="2"/>
+        <v>13946239.632609431</v>
+      </c>
+      <c r="F62" s="5">
+        <f t="shared" si="3"/>
+        <v>19854507.696011167</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="7">
+        <v>46</v>
+      </c>
+      <c r="C63" s="14">
+        <f t="shared" si="0"/>
+        <v>911133413.75087261</v>
+      </c>
+      <c r="D63" s="14">
+        <f t="shared" si="1"/>
+        <v>23325015.392022338</v>
+      </c>
+      <c r="E63" s="14">
+        <f t="shared" si="2"/>
+        <v>19854507.696011167</v>
+      </c>
+      <c r="F63" s="5">
+        <f t="shared" si="3"/>
+        <v>28265789.649077542</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" s="7">
+        <v>47</v>
+      </c>
+      <c r="C64" s="14">
+        <f t="shared" si="0"/>
+        <v>1297131402.5833104</v>
+      </c>
+      <c r="D64" s="14">
+        <f t="shared" si="1"/>
+        <v>33206563.906132746</v>
+      </c>
+      <c r="E64" s="14">
+        <f t="shared" si="2"/>
+        <v>28265789.649077542</v>
+      </c>
+      <c r="F64" s="5">
+        <f t="shared" si="3"/>
+        <v>40240477.21145016</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65" s="7">
+        <v>48</v>
+      </c>
+      <c r="C65" s="14">
+        <f t="shared" si="0"/>
+        <v>1846655879.5612333</v>
+      </c>
+      <c r="D65" s="14">
+        <f t="shared" si="1"/>
+        <v>47274390.516767569</v>
+      </c>
+      <c r="E65" s="14">
+        <f t="shared" si="2"/>
+        <v>40240477.21145016</v>
+      </c>
+      <c r="F65" s="5">
+        <f t="shared" si="3"/>
+        <v>57288192.769738719</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="7">
+        <v>49</v>
+      </c>
+      <c r="C66" s="14">
+        <f t="shared" si="0"/>
+        <v>2628984180.574604</v>
+      </c>
+      <c r="D66" s="14">
+        <f t="shared" si="1"/>
+        <v>67301995.022709861</v>
+      </c>
+      <c r="E66" s="14">
+        <f t="shared" si="2"/>
+        <v>57288192.769738719</v>
+      </c>
+      <c r="F66" s="5">
+        <f t="shared" si="3"/>
+        <v>81558104.134234518</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="7">
+        <v>50</v>
+      </c>
+      <c r="C67" s="14">
+        <f t="shared" si="0"/>
+        <v>3742742704.9124675</v>
+      </c>
+      <c r="D67" s="14">
+        <f t="shared" si="1"/>
+        <v>95814213.245759174</v>
+      </c>
+      <c r="E67" s="14">
+        <f t="shared" si="2"/>
+        <v>81558104.134234518</v>
+      </c>
+      <c r="F67" s="5">
+        <f t="shared" si="3"/>
+        <v>116109865.37324104</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68" s="7">
+        <v>51</v>
+      </c>
+      <c r="C68" s="14">
+        <f t="shared" si="0"/>
+        <v>5328340527.3719873</v>
+      </c>
+      <c r="D68" s="14">
+        <f t="shared" si="1"/>
+        <v>136405517.50072289</v>
+      </c>
+      <c r="E68" s="14">
+        <f t="shared" si="2"/>
+        <v>116109865.37324104</v>
+      </c>
+      <c r="F68" s="5">
+        <f t="shared" si="3"/>
+        <v>165299340.63699272</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="7">
+        <v>52</v>
+      </c>
+      <c r="C69" s="14">
+        <f t="shared" si="0"/>
+        <v>7585670459.8930693</v>
+      </c>
+      <c r="D69" s="14">
+        <f t="shared" si="1"/>
+        <v>194193163.77326256</v>
+      </c>
+      <c r="E69" s="14">
+        <f t="shared" si="2"/>
+        <v>165299340.63699272</v>
+      </c>
+      <c r="F69" s="5">
+        <f t="shared" si="3"/>
+        <v>235327738.32086176</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="7">
+        <v>53</v>
+      </c>
+      <c r="C70" s="14">
+        <f t="shared" si="0"/>
+        <v>10799309096.424255</v>
+      </c>
+      <c r="D70" s="14">
+        <f t="shared" si="1"/>
+        <v>276462312.86846095</v>
+      </c>
+      <c r="E70" s="14">
+        <f t="shared" si="2"/>
+        <v>235327738.32086176</v>
+      </c>
+      <c r="F70" s="5">
+        <f t="shared" si="3"/>
+        <v>335023383.69774818</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="7">
+        <v>54</v>
+      </c>
+      <c r="C71" s="14">
+        <f t="shared" si="0"/>
+        <v>15374392754.962318</v>
+      </c>
+      <c r="D71" s="14">
+        <f t="shared" si="1"/>
+        <v>393584454.52703536</v>
+      </c>
+      <c r="E71" s="14">
+        <f t="shared" si="2"/>
+        <v>335023383.69774818</v>
+      </c>
+      <c r="F71" s="5">
+        <f t="shared" si="3"/>
+        <v>476954686.36702764</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="7">
+        <v>55</v>
+      </c>
+      <c r="C72" s="14">
+        <f t="shared" si="0"/>
+        <v>21887692117.461716</v>
+      </c>
+      <c r="D72" s="14">
+        <f t="shared" si="1"/>
+        <v>560324918.20701993</v>
+      </c>
+      <c r="E72" s="14">
+        <f t="shared" si="2"/>
+        <v>476954686.36702764</v>
+      </c>
+      <c r="F72" s="5">
+        <f t="shared" si="3"/>
+        <v>679014611.86572921</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73" s="7">
+        <v>56</v>
+      </c>
+      <c r="C73" s="14">
+        <f t="shared" si="0"/>
+        <v>31160324434.548378</v>
+      </c>
+      <c r="D73" s="14">
+        <f t="shared" si="1"/>
+        <v>797704305.5244385</v>
+      </c>
+      <c r="E73" s="14">
+        <f t="shared" si="2"/>
+        <v>679014611.86572921</v>
+      </c>
+      <c r="F73" s="5">
+        <f t="shared" si="3"/>
+        <v>966676408.27491498</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" s="7">
+        <v>57</v>
+      </c>
+      <c r="C74" s="14">
+        <f t="shared" si="0"/>
+        <v>44361269961.929359</v>
+      </c>
+      <c r="D74" s="14">
+        <f t="shared" si="1"/>
+        <v>1135648511.0253916</v>
+      </c>
+      <c r="E74" s="14">
+        <f t="shared" si="2"/>
+        <v>966676408.27491498</v>
+      </c>
+      <c r="F74" s="5">
+        <f t="shared" si="3"/>
+        <v>1376204962.2874308</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="7">
+        <v>58</v>
+      </c>
+      <c r="C75" s="14">
+        <f t="shared" si="0"/>
+        <v>63154742716.776161</v>
+      </c>
+      <c r="D75" s="14">
+        <f t="shared" si="1"/>
+        <v>1616761413.5494697</v>
+      </c>
+      <c r="E75" s="14">
+        <f t="shared" si="2"/>
+        <v>1376204962.2874308</v>
+      </c>
+      <c r="F75" s="5">
+        <f t="shared" si="3"/>
+        <v>1959228633.2966213</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="7">
+        <v>59</v>
+      </c>
+      <c r="C76" s="14">
+        <f t="shared" si="0"/>
+        <v>89909994259.522369</v>
+      </c>
+      <c r="D76" s="14">
+        <f t="shared" si="1"/>
+        <v>2301695853.0437727</v>
+      </c>
+      <c r="E76" s="14">
+        <f t="shared" si="2"/>
+        <v>1959228633.2966213</v>
+      </c>
+      <c r="F76" s="5">
+        <f t="shared" si="3"/>
+        <v>2789247926.5218859</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="7">
+        <v>60</v>
+      </c>
+      <c r="C77" s="14">
+        <f t="shared" si="0"/>
+        <v>127999999999.99998</v>
+      </c>
+      <c r="D77" s="14">
+        <f t="shared" si="1"/>
+        <v>3276799999.9999995</v>
+      </c>
+      <c r="E77" s="14">
+        <f t="shared" si="2"/>
+        <v>2789247926.5218859</v>
+      </c>
+      <c r="F77" s="5">
+        <f t="shared" si="3"/>
+        <v>3970901539.2022333</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78" s="7">
+        <v>61</v>
+      </c>
+      <c r="C78" s="14">
+        <f t="shared" si="0"/>
+        <v>182226682750.1745</v>
+      </c>
+      <c r="D78" s="14">
+        <f t="shared" si="1"/>
+        <v>4665003078.4044676</v>
+      </c>
+      <c r="E78" s="14">
+        <f t="shared" si="2"/>
+        <v>3970901539.2022333</v>
+      </c>
+      <c r="F78" s="5">
+        <f t="shared" si="3"/>
+        <v>5653157929.8155079</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="7">
+        <v>62</v>
+      </c>
+      <c r="C79" s="14">
+        <f t="shared" si="0"/>
+        <v>259426280516.66205</v>
+      </c>
+      <c r="D79" s="14">
+        <f t="shared" si="1"/>
+        <v>6641312781.2265482</v>
+      </c>
+      <c r="E79" s="14">
+        <f t="shared" si="2"/>
+        <v>5653157929.8155079</v>
+      </c>
+      <c r="F79" s="5">
+        <f t="shared" si="3"/>
+        <v>8048095442.2900314</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B80" s="8">
+        <v>63</v>
+      </c>
+      <c r="C80" s="9">
+        <f t="shared" si="0"/>
+        <v>369331175912.24664</v>
+      </c>
+      <c r="D80" s="9">
+        <f t="shared" si="1"/>
+        <v>9454878103.3535137</v>
+      </c>
+      <c r="E80" s="9">
+        <f t="shared" si="2"/>
+        <v>8048095442.2900314</v>
+      </c>
+      <c r="F80" s="6">
+        <f t="shared" si="3"/>
+        <v>4727439051.6767569</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81" s="13"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B17:F17">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$B$17&lt;$B$9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18:F49">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="B18:F80">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$B18&lt;$B$9</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>